<commit_message>
[modify] 30030 / 40071 [template] 40150
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40150.xlsx
+++ b/PhoenixCI/Excel_Template/40150.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Source\Repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJSOFT\source\repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{195B7872-24F6-4376-9690-D783187CED38}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA18917D-5AA1-4233-B1A6-708C5E4EF0FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="14895" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DPSR&amp;SC" sheetId="1" r:id="rId1"/>
     <sheet name="VSR" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,54 +39,64 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="11"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>股價指數類選擇權契約</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t>臺指選擇權</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t>(TXO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>代號</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t>電子選擇權</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
+      <t>(TEO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>波動度偵測全距</t>
+      <t>金融選擇權</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(TFO)</t>
     </r>
   </si>
   <si>
@@ -99,7 +108,7 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>臺指選擇權</t>
+      <t>非金電選擇權</t>
     </r>
     <r>
       <rPr>
@@ -108,7 +117,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(TXO)</t>
+      <t>(XIO)</t>
     </r>
   </si>
   <si>
@@ -120,7 +129,7 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>電子選擇權</t>
+      <t>櫃買選擇權</t>
     </r>
     <r>
       <rPr>
@@ -129,49 +138,33 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(TEO)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t>(GTO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>金融選擇權</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(TFO)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t>股票選擇權契約</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>非金電選擇權</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(XIO)</t>
+      <t>波動度偵測全距</t>
     </r>
   </si>
   <si>
@@ -183,7 +176,7 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>櫃買選擇權</t>
+      <t>黃金選擇權</t>
     </r>
     <r>
       <rPr>
@@ -192,56 +185,82 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(GTO)</t>
+      <t>(TGO)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>股票選擇權契約</t>
+      <t>波動度偵測全距</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>波動度偵測全距</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
+      <t>股價指數類選擇權契約</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>標的證券為股票之股票選擇權</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+      <t>代號</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(STC)</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>標的證券為股票之股票選擇權</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>標的證券為受益憑證之股票選擇權</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品類選擇權契約(代號)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>匯率類選擇權契約(代號)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -252,7 +271,7 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>標的證券為受益憑證之股票選擇權</t>
+      <t>美元兌人民幣匯率選擇權</t>
     </r>
     <r>
       <rPr>
@@ -261,33 +280,20 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(ETC)</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+      <t>(RHO)</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="標楷體"/>
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>黃金選擇權契約</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>黃金選擇權</t>
+      <t>小型美元兌人民幣匯率選擇權</t>
     </r>
     <r>
       <rPr>
@@ -296,66 +302,9 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>(TGO)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>匯率選擇權契約</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>美元兌人民幣選擇權</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(RHO)</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>小型美元兌人民幣選擇權</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>(RTO)</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -375,19 +324,6 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="1"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="標楷體"/>
-      <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
@@ -436,6 +372,21 @@
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
@@ -499,53 +450,50 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -898,16 +846,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -1223,106 +1171,106 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.25" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="6"/>
+    <col min="1" max="1" width="35.25" style="5" customWidth="1"/>
+    <col min="2" max="2" width="39.25" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="12"/>
-    </row>
-    <row r="9" spans="1:2" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>10</v>
+      <c r="B12" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="14"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>